<commit_message>
added more test cases for array
</commit_message>
<xml_diff>
--- a/src/test/resources/Exceldata/dsAlgoData.xlsx
+++ b/src/test/resources/Exceldata/dsAlgoData.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="11110"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="11207"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/maya/git/DSALGO_BDD/src/test/resources/Exceldata/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/maya/eclipse-workspace/DSAlgoQualityQuesters/src/test/resources/Exceldata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52D7B0D1-5F5B-A448-BBB7-564022672637}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B414BC6C-A112-2945-8324-3CBB2C54967B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4700" yWindow="2860" windowWidth="17280" windowHeight="8880" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="740" windowWidth="29400" windowHeight="16740" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Register" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="16">
   <si>
     <t>username</t>
   </si>
@@ -73,9 +73,6 @@
   </si>
   <si>
     <t>Element Found</t>
-  </si>
-  <si>
-    <t>submission success</t>
   </si>
   <si>
     <t>def findMaxConsecutiveOnes(nums) :
@@ -132,6 +129,21 @@
   </si>
   <si>
     <t>[4, 9, 9, 49, 121]</t>
+  </si>
+  <si>
+    <t>Submission Successful</t>
+  </si>
+  <si>
+    <t>def search(input_list, num):
+if(num in input_list):
+output = ("Element Found")
+\b
+\b
+else:
+output = ("Not Found")
+\b
+\b
+return(output)</t>
   </si>
 </sst>
 </file>
@@ -510,7 +522,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2:B2"/>
     </sheetView>
   </sheetViews>
@@ -540,7 +552,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:B11"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
@@ -583,58 +597,58 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
-        <v>7</v>
+        <v>15</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" s="3" t="s">
         <v>10</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B10" s="3" t="s">
         <v>13</v>
-      </c>
-      <c r="B10" s="3" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
changes for array module
</commit_message>
<xml_diff>
--- a/src/test/resources/Exceldata/dsAlgoData.xlsx
+++ b/src/test/resources/Exceldata/dsAlgoData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/maya/eclipse-workspace/DSAlgoQualityQuesters/src/test/resources/Exceldata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B414BC6C-A112-2945-8324-3CBB2C54967B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C00EC8B-FB8B-3849-AD9B-C53FD84C4E0B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="740" windowWidth="29400" windowHeight="16740" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="740" windowWidth="29400" windowHeight="16680" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Register" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="18">
   <si>
     <t>username</t>
   </si>
@@ -144,6 +144,28 @@
 \b
 \b
 return(output)</t>
+  </si>
+  <si>
+    <t>def findMaxConsecutiveOnes(nums) :
+max_count = 0
+current_count = 0
+for num in nums:
+if num == 1:
+current_count += 1
+max_count = max(max_count, current_count)
+\b
+\b
+else:
+current_count = 0
+#\b\b\b
+\b
+\b
+\b
+\b
+return max_count</t>
+  </si>
+  <si>
+    <t>def findNumbers(nums):return sum(len(str(num)) % 2 == 0 for num in nums)</t>
   </si>
 </sst>
 </file>
@@ -553,7 +575,7 @@
   <dimension ref="A1:B11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -613,7 +635,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="B7" s="3" t="s">
         <v>14</v>
@@ -629,7 +651,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="B9" s="3" t="s">
         <v>14</v>

</xml_diff>

<commit_message>
added login features scenarios
</commit_message>
<xml_diff>
--- a/src/test/resources/Exceldata/dsAlgoData.xlsx
+++ b/src/test/resources/Exceldata/dsAlgoData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/maya/eclipse-workspace/DSAlgoQualityQuesters/src/test/resources/Exceldata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C00EC8B-FB8B-3849-AD9B-C53FD84C4E0B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5486E3B-E465-3040-ACCB-E6B7F581FE18}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="740" windowWidth="29400" windowHeight="16680" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="740" windowWidth="29400" windowHeight="16680" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Register" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="23">
   <si>
     <t>username</t>
   </si>
@@ -166,6 +166,21 @@
   </si>
   <si>
     <t>def findNumbers(nums):return sum(len(str(num)) % 2 == 0 for num in nums)</t>
+  </si>
+  <si>
+    <t>numpy</t>
+  </si>
+  <si>
+    <t>expectedmessage</t>
+  </si>
+  <si>
+    <t>user</t>
+  </si>
+  <si>
+    <t>sdet185</t>
+  </si>
+  <si>
+    <t>Invalid Username and Password</t>
   </si>
 </sst>
 </file>
@@ -221,17 +236,18 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -532,8 +548,8 @@
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B4" s="5"/>
-      <c r="C4" s="5"/>
+      <c r="B4" s="4"/>
+      <c r="C4" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -542,28 +558,56 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:B2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="21.1640625" customWidth="1"/>
     <col min="2" max="2" width="17.1640625" customWidth="1"/>
+    <col min="3" max="3" width="25.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B2" s="4"/>
+      <c r="C1" s="5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="A2" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4" s="5"/>
+      <c r="B4" s="5"/>
+      <c r="C4" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -574,7 +618,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:B11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Data driven for Registration Scenario
</commit_message>
<xml_diff>
--- a/src/test/resources/Exceldata/dsAlgoData.xlsx
+++ b/src/test/resources/Exceldata/dsAlgoData.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="11207"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="28227"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/maya/eclipse-workspace/DSAlgoQualityQuesters/src/test/resources/Exceldata/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Rajasri\Numpy Ninja\eclipse-workspace\DSALGO_BDD\src\test\resources\Exceldata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5486E3B-E465-3040-ACCB-E6B7F581FE18}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A619E7A0-05E1-44CF-B465-8E850AFA8FA6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="740" windowWidth="29400" windowHeight="16680" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Register" sheetId="1" r:id="rId1"/>
@@ -26,8 +26,6 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -35,15 +33,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="52">
   <si>
     <t>username</t>
   </si>
   <si>
     <t>password</t>
-  </si>
-  <si>
-    <t>confirmpwd</t>
   </si>
   <si>
     <t>PythonCode</t>
@@ -182,12 +177,142 @@
   <si>
     <t>Invalid Username and Password</t>
   </si>
+  <si>
+    <t>Verify that user received error message for empty username field</t>
+  </si>
+  <si>
+    <t>passwordConfirmation</t>
+  </si>
+  <si>
+    <t>skdfsd</t>
+  </si>
+  <si>
+    <t>skdfsd1</t>
+  </si>
+  <si>
+    <t>Verify that user receives error message for empty Password field during registration</t>
+  </si>
+  <si>
+    <t>jack</t>
+  </si>
+  <si>
+    <t>Verify that user received error message for empty username field (gave username for mandatory purpose to execute the code)</t>
+  </si>
+  <si>
+    <t>Jack</t>
+  </si>
+  <si>
+    <t>comments/Scenario ref</t>
+  </si>
+  <si>
+    <t>Verify that user receives error message for empty Password Confirmation field during registration</t>
+  </si>
+  <si>
+    <t>Verify that user receives error message for invalid username field during registration</t>
+  </si>
+  <si>
+    <t>@&amp;%^&amp;</t>
+  </si>
+  <si>
+    <t>Leon</t>
+  </si>
+  <si>
+    <t>Verify that user receives error message for invalid password field during registration</t>
+  </si>
+  <si>
+    <t>ann</t>
+  </si>
+  <si>
+    <t>Verify that user receives error message for mismatched Password and Password Confirmation field during registration</t>
+  </si>
+  <si>
+    <t>leon</t>
+  </si>
+  <si>
+    <t>onel</t>
+  </si>
+  <si>
+    <t>Rose</t>
+  </si>
+  <si>
+    <t>Verify that user is able to land on Homepage after registration with valid fields (Since it's a valid scenario commenting in feature)</t>
+  </si>
+  <si>
+    <t>Algo24</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Verify that the user receives the error message for entering username less than </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF008000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>8</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> characters</t>
+    </r>
+  </si>
+  <si>
+    <t>@SDET!</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Verify that the user receives the error message for entering password less than </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF008000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>8</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> characters</t>
+    </r>
+  </si>
+  <si>
+    <t>SDET185</t>
+  </si>
+  <si>
+    <t>abc</t>
+  </si>
+  <si>
+    <t>NA</t>
+  </si>
+  <si>
+    <t>1234</t>
+  </si>
+  <si>
+    <t>54231</t>
+  </si>
+  <si>
+    <t>11</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="7">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -204,9 +329,33 @@
     </font>
     <font>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF008000"/>
+      <name val="Consolas"/>
+      <family val="3"/>
     </font>
   </fonts>
   <fills count="3">
@@ -234,20 +383,27 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -524,35 +680,176 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:D11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:C6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="2" width="18" customWidth="1"/>
-    <col min="3" max="3" width="15.33203125" customWidth="1"/>
+    <col min="3" max="3" width="21.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="126.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B4" s="4"/>
-      <c r="C4" s="4"/>
+      <c r="C1" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="D1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="B2" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="C2" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="B3" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="C3" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="D3" s="6" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="B4" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="C4" s="12" t="s">
+        <v>48</v>
+      </c>
+      <c r="D4" s="6" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="B5" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="C5" s="13" t="s">
+        <v>48</v>
+      </c>
+      <c r="D5" s="6" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="B6" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="C6" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="D6" s="6" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="A7" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="B7" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="C7" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="D7" s="6" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
+      <c r="A8" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="B8" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="C8" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="D8" s="6" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
+      <c r="A9" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="B9" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="C9" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="D9" s="7" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4">
+      <c r="A10" s="9" t="s">
+        <v>51</v>
+      </c>
+      <c r="B10" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="C10" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="D10" s="6" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4">
+      <c r="A11" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="B11" s="9" t="s">
+        <v>51</v>
+      </c>
+      <c r="C11" s="9" t="s">
+        <v>51</v>
+      </c>
+      <c r="D11" s="6" t="s">
+        <v>45</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -560,54 +857,54 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="21.1640625" customWidth="1"/>
-    <col min="2" max="2" width="17.1640625" customWidth="1"/>
-    <col min="3" max="3" width="25.1640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="21.109375" customWidth="1"/>
+    <col min="2" max="2" width="17.109375" customWidth="1"/>
+    <col min="3" max="3" width="25.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="C1" s="4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B2" s="5" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A2" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="B2" s="6" t="s">
+      <c r="C2" s="4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C2" s="5" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A3" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="B3" s="5" t="s">
+      <c r="C3" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="C3" s="5" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A4" s="5"/>
-      <c r="B4" s="5"/>
-      <c r="C4" s="5"/>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4" s="4"/>
+      <c r="B4" s="4"/>
+      <c r="C4" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -622,99 +919,99 @@
       <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="104.5" customWidth="1"/>
+    <col min="1" max="1" width="104.44140625" customWidth="1"/>
     <col min="2" max="2" width="17.33203125" customWidth="1"/>
-    <col min="3" max="3" width="19.1640625" customWidth="1"/>
+    <col min="3" max="3" width="19.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2">
       <c r="A1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="1" t="s">
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" s="1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A2" s="1" t="s">
+      <c r="B2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="1" t="s">
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" s="2" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A3" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A4" s="2" t="s">
+      <c r="B4" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B4" s="1" t="s">
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6" s="2" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A5" s="2" t="s">
+      <c r="B6" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="B5" s="3" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A6" s="2" t="s">
+      <c r="B7" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2">
+      <c r="A8" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B8" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B6" s="3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A7" s="2" t="s">
+    </row>
+    <row r="9" spans="1:2">
+      <c r="A9" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B7" s="3" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A8" s="2" t="s">
+      <c r="B9" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2">
+      <c r="A10" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B8" s="3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A9" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="B9" s="3" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A10" s="2" t="s">
+      <c r="B10" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B10" s="3" t="s">
+    </row>
+    <row r="11" spans="1:2">
+      <c r="A11" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B11" s="3" t="s">
         <v>13</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A11" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="B11" s="3" t="s">
-        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
changes to read the password from excelsheet
</commit_message>
<xml_diff>
--- a/src/test/resources/Exceldata/dsAlgoData.xlsx
+++ b/src/test/resources/Exceldata/dsAlgoData.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="28227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="11207"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Rajasri\Numpy Ninja\eclipse-workspace\DSALGO_BDD\src\test\resources\Exceldata\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/maya/git/DSALGO_BDD/src/test/resources/Exceldata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A619E7A0-05E1-44CF-B465-8E850AFA8FA6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FADB6962-DEE3-5949-9CE3-B1835DD51679}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="740" windowWidth="23260" windowHeight="12460" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Register" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="55">
   <si>
     <t>username</t>
   </si>
@@ -307,12 +307,21 @@
   <si>
     <t>11</t>
   </si>
+  <si>
+    <t>maya</t>
+  </si>
+  <si>
+    <t>babuji_123</t>
+  </si>
+  <si>
+    <t>You are looged in</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -385,7 +394,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
@@ -404,6 +413,7 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -682,18 +692,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="2" width="18" customWidth="1"/>
     <col min="3" max="3" width="21.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="126.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="126.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -707,7 +717,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" s="8" t="s">
         <v>47</v>
       </c>
@@ -721,7 +731,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" s="8" t="s">
         <v>47</v>
       </c>
@@ -735,7 +745,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" s="10" t="s">
         <v>27</v>
       </c>
@@ -749,7 +759,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="5" spans="1:4">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" s="8" t="s">
         <v>29</v>
       </c>
@@ -763,7 +773,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="6" spans="1:4">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" s="10" t="s">
         <v>33</v>
       </c>
@@ -777,7 +787,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="7" spans="1:4">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" s="10" t="s">
         <v>36</v>
       </c>
@@ -791,7 +801,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="8" spans="1:4">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" s="9" t="s">
         <v>40</v>
       </c>
@@ -805,7 +815,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="9" spans="1:4">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" s="10" t="s">
         <v>29</v>
       </c>
@@ -819,7 +829,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="10" spans="1:4">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" s="9" t="s">
         <v>51</v>
       </c>
@@ -833,7 +843,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="11" spans="1:4">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" s="10" t="s">
         <v>46</v>
       </c>
@@ -857,18 +867,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="21.109375" customWidth="1"/>
-    <col min="2" max="2" width="17.109375" customWidth="1"/>
-    <col min="3" max="3" width="25.109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="21.1640625" customWidth="1"/>
+    <col min="2" max="2" width="17.1640625" customWidth="1"/>
+    <col min="3" max="3" width="25.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -879,7 +889,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
         <v>17</v>
       </c>
@@ -890,7 +900,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
         <v>0</v>
       </c>
@@ -901,10 +911,16 @@
         <v>21</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
-      <c r="A4" s="4"/>
-      <c r="B4" s="4"/>
-      <c r="C4" s="4"/>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4" s="14" t="s">
+        <v>52</v>
+      </c>
+      <c r="B4" s="14" t="s">
+        <v>53</v>
+      </c>
+      <c r="C4" s="14" t="s">
+        <v>54</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -919,14 +935,14 @@
       <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="104.44140625" customWidth="1"/>
+    <col min="1" max="1" width="104.5" customWidth="1"/>
     <col min="2" max="2" width="17.33203125" customWidth="1"/>
-    <col min="3" max="3" width="19.109375" customWidth="1"/>
+    <col min="3" max="3" width="19.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -934,7 +950,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>4</v>
       </c>
@@ -942,7 +958,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>5</v>
       </c>
@@ -950,7 +966,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>6</v>
       </c>
@@ -958,7 +974,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
         <v>14</v>
       </c>
@@ -966,7 +982,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="1:2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
         <v>8</v>
       </c>
@@ -974,7 +990,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:2">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
         <v>15</v>
       </c>
@@ -982,7 +998,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="1:2">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
         <v>10</v>
       </c>
@@ -990,7 +1006,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="9" spans="1:2">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
         <v>16</v>
       </c>
@@ -998,7 +1014,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="10" spans="1:2">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
         <v>11</v>
       </c>
@@ -1006,7 +1022,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="11" spans="1:2">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
         <v>11</v>
       </c>

</xml_diff>

<commit_message>
Removed url in config related to LL feature
</commit_message>
<xml_diff>
--- a/src/test/resources/Exceldata/dsAlgoData.xlsx
+++ b/src/test/resources/Exceldata/dsAlgoData.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="11207"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="28227"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/maya/git/DSALGO_BDD/src/test/resources/Exceldata/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Rajasri\Numpy Ninja\eclipse-workspace\DSALGO_BDD\src\test\resources\Exceldata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23F3B98D-6F8D-534F-80D0-DC3CAD2BEE6B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F5E504E-2BAD-461A-A3E0-5B9CB82A82DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="740" windowWidth="23260" windowHeight="12460" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2688" yWindow="2688" windowWidth="17280" windowHeight="8880" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Register" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="57">
   <si>
     <t>username</t>
   </si>
@@ -316,17 +316,30 @@
   <si>
     <t>You are logged in</t>
   </si>
+  <si>
+    <t>@SDET!*%</t>
+  </si>
+  <si>
+    <t>Vaid username and password</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -392,27 +405,28 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
@@ -696,14 +710,14 @@
       <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="2" width="18" customWidth="1"/>
     <col min="3" max="3" width="21.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="126.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="126.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -717,7 +731,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4">
       <c r="A2" s="8" t="s">
         <v>47</v>
       </c>
@@ -731,7 +745,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4">
       <c r="A3" s="8" t="s">
         <v>47</v>
       </c>
@@ -745,7 +759,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4">
       <c r="A4" s="10" t="s">
         <v>27</v>
       </c>
@@ -759,7 +773,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:4">
       <c r="A5" s="8" t="s">
         <v>29</v>
       </c>
@@ -773,7 +787,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:4">
       <c r="A6" s="10" t="s">
         <v>33</v>
       </c>
@@ -787,7 +801,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:4">
       <c r="A7" s="10" t="s">
         <v>36</v>
       </c>
@@ -801,7 +815,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:4">
       <c r="A8" s="9" t="s">
         <v>40</v>
       </c>
@@ -815,7 +829,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:4">
       <c r="A9" s="10" t="s">
         <v>29</v>
       </c>
@@ -829,7 +843,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:4">
       <c r="A10" s="9" t="s">
         <v>51</v>
       </c>
@@ -843,7 +857,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:4">
       <c r="A11" s="10" t="s">
         <v>46</v>
       </c>
@@ -865,20 +879,20 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="21.1640625" customWidth="1"/>
-    <col min="2" max="2" width="17.1640625" customWidth="1"/>
-    <col min="3" max="3" width="25.1640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="21.109375" customWidth="1"/>
+    <col min="2" max="2" width="17.109375" customWidth="1"/>
+    <col min="3" max="3" width="25.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -889,7 +903,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3">
       <c r="A2" s="4" t="s">
         <v>17</v>
       </c>
@@ -900,7 +914,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3">
       <c r="A3" s="4" t="s">
         <v>0</v>
       </c>
@@ -911,7 +925,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3">
       <c r="A4" s="14" t="s">
         <v>52</v>
       </c>
@@ -920,6 +934,17 @@
       </c>
       <c r="C4" s="14" t="s">
         <v>54</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="C5" s="15" t="s">
+        <v>56</v>
       </c>
     </row>
   </sheetData>
@@ -935,14 +960,14 @@
       <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="104.5" customWidth="1"/>
+    <col min="1" max="1" width="104.44140625" customWidth="1"/>
     <col min="2" max="2" width="17.33203125" customWidth="1"/>
-    <col min="3" max="3" width="19.1640625" customWidth="1"/>
+    <col min="3" max="3" width="19.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -950,7 +975,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2">
       <c r="A2" s="1" t="s">
         <v>4</v>
       </c>
@@ -958,7 +983,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:2">
       <c r="A3" s="1" t="s">
         <v>5</v>
       </c>
@@ -966,7 +991,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:2">
       <c r="A4" s="2" t="s">
         <v>6</v>
       </c>
@@ -974,7 +999,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:2">
       <c r="A5" s="2" t="s">
         <v>14</v>
       </c>
@@ -982,7 +1007,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:2">
       <c r="A6" s="2" t="s">
         <v>8</v>
       </c>
@@ -990,7 +1015,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:2">
       <c r="A7" s="2" t="s">
         <v>15</v>
       </c>
@@ -998,7 +1023,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:2">
       <c r="A8" s="2" t="s">
         <v>10</v>
       </c>
@@ -1006,7 +1031,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:2">
       <c r="A9" s="2" t="s">
         <v>16</v>
       </c>
@@ -1014,7 +1039,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:2">
       <c r="A10" s="2" t="s">
         <v>11</v>
       </c>
@@ -1022,7 +1047,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:2">
       <c r="A11" s="2" t="s">
         <v>11</v>
       </c>

</xml_diff>

<commit_message>
Updated Stack,LL to use data from excel
</commit_message>
<xml_diff>
--- a/src/test/resources/Exceldata/dsAlgoData.xlsx
+++ b/src/test/resources/Exceldata/dsAlgoData.xlsx
@@ -8,14 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Rajasri\Numpy Ninja\eclipse-workspace\DSALGO_BDD\src\test\resources\Exceldata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F5E504E-2BAD-461A-A3E0-5B9CB82A82DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC8B15B9-B856-43F8-949D-F7ABF891A2CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2688" yWindow="2688" windowWidth="17280" windowHeight="8880" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Register" sheetId="1" r:id="rId1"/>
     <sheet name="SignIn" sheetId="2" r:id="rId2"/>
     <sheet name="PythonCode" sheetId="3" r:id="rId3"/>
+    <sheet name="SubPage" sheetId="4" r:id="rId4"/>
+    <sheet name="StackSubPage" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -33,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="72">
   <si>
     <t>username</t>
   </si>
@@ -322,17 +324,69 @@
   <si>
     <t>Vaid username and password</t>
   </si>
+  <si>
+    <t>print("Welcome")</t>
+  </si>
+  <si>
+    <t>Welcome</t>
+  </si>
+  <si>
+    <t>print(Day')</t>
+  </si>
+  <si>
+    <t>Introduction</t>
+  </si>
+  <si>
+    <t>Creating Linked LIst</t>
+  </si>
+  <si>
+    <t>Types of Linked List</t>
+  </si>
+  <si>
+    <t>Implement Linked List in Python</t>
+  </si>
+  <si>
+    <t>Traversal</t>
+  </si>
+  <si>
+    <t>Insertion</t>
+  </si>
+  <si>
+    <t>Deletion</t>
+  </si>
+  <si>
+    <t>SubPage</t>
+  </si>
+  <si>
+    <t>OperationsInStack</t>
+  </si>
+  <si>
+    <t>Implementation</t>
+  </si>
+  <si>
+    <t>Applications</t>
+  </si>
+  <si>
+    <t>Page</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8">
+  <fonts count="9">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -394,7 +448,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -402,31 +456,48 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
-    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
@@ -724,7 +795,7 @@
       <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="C1" s="3" t="s">
         <v>23</v>
       </c>
       <c r="D1" t="s">
@@ -732,142 +803,142 @@
       </c>
     </row>
     <row r="2" spans="1:4">
-      <c r="A2" s="8" t="s">
+      <c r="A2" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="B2" s="10" t="s">
+      <c r="B2" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="C2" s="10" t="s">
+      <c r="C2" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="D2" s="6" t="s">
+      <c r="D2" s="3" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="3" spans="1:4">
-      <c r="A3" s="8" t="s">
+      <c r="A3" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="B3" s="10" t="s">
+      <c r="B3" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="C3" s="10" t="s">
+      <c r="C3" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="D3" s="6" t="s">
+      <c r="D3" s="3" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="4" spans="1:4">
-      <c r="A4" s="10" t="s">
+      <c r="A4" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="B4" s="11" t="s">
+      <c r="B4" s="8" t="s">
         <v>48</v>
       </c>
-      <c r="C4" s="12" t="s">
+      <c r="C4" s="9" t="s">
         <v>48</v>
       </c>
-      <c r="D4" s="6" t="s">
+      <c r="D4" s="3" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="5" spans="1:4">
-      <c r="A5" s="8" t="s">
+      <c r="A5" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="B5" s="8" t="s">
+      <c r="B5" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="C5" s="13" t="s">
+      <c r="C5" s="10" t="s">
         <v>48</v>
       </c>
-      <c r="D5" s="6" t="s">
+      <c r="D5" s="3" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="6" spans="1:4">
-      <c r="A6" s="10" t="s">
+      <c r="A6" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="B6" s="9" t="s">
+      <c r="B6" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="C6" s="9" t="s">
+      <c r="C6" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="D6" s="6" t="s">
+      <c r="D6" s="3" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="7" spans="1:4">
-      <c r="A7" s="10" t="s">
+      <c r="A7" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="B7" s="9" t="s">
+      <c r="B7" s="6" t="s">
         <v>50</v>
       </c>
-      <c r="C7" s="9" t="s">
+      <c r="C7" s="6" t="s">
         <v>50</v>
       </c>
-      <c r="D7" s="6" t="s">
+      <c r="D7" s="3" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="8" spans="1:4">
-      <c r="A8" s="9" t="s">
+      <c r="A8" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="B8" s="10" t="s">
+      <c r="B8" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="C8" s="10" t="s">
+      <c r="C8" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="D8" s="6" t="s">
+      <c r="D8" s="3" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="9" spans="1:4">
-      <c r="A9" s="10" t="s">
+      <c r="A9" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="B9" s="10" t="s">
+      <c r="B9" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="C9" s="10" t="s">
+      <c r="C9" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="D9" s="7" t="s">
+      <c r="D9" s="4" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="10" spans="1:4">
-      <c r="A10" s="9" t="s">
+      <c r="A10" s="6" t="s">
         <v>51</v>
       </c>
-      <c r="B10" s="10" t="s">
+      <c r="B10" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="C10" s="10" t="s">
+      <c r="C10" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="D10" s="6" t="s">
+      <c r="D10" s="3" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="11" spans="1:4">
-      <c r="A11" s="10" t="s">
+      <c r="A11" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="B11" s="9" t="s">
+      <c r="B11" s="6" t="s">
         <v>51</v>
       </c>
-      <c r="C11" s="9" t="s">
+      <c r="C11" s="6" t="s">
         <v>51</v>
       </c>
-      <c r="D11" s="6" t="s">
+      <c r="D11" s="3" t="s">
         <v>45</v>
       </c>
     </row>
@@ -881,7 +952,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:C5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
@@ -899,51 +970,51 @@
       <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C1" s="1" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="2" spans="1:3">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="B2" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="C2" s="1" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="3" spans="1:3">
-      <c r="A3" s="4" t="s">
+      <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="B3" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="C3" s="1" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="4" spans="1:3">
-      <c r="A4" s="14" t="s">
+      <c r="A4" s="11" t="s">
         <v>52</v>
       </c>
-      <c r="B4" s="14" t="s">
+      <c r="B4" s="11" t="s">
         <v>53</v>
       </c>
-      <c r="C4" s="14" t="s">
+      <c r="C4" s="11" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="5" spans="1:3">
-      <c r="A5" s="7" t="s">
+      <c r="A5" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="B5" s="7" t="s">
+      <c r="B5" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="C5" s="15" t="s">
+      <c r="C5" s="12" t="s">
         <v>56</v>
       </c>
     </row>
@@ -954,7 +1025,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:B11"/>
+  <dimension ref="A1:B13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A9" sqref="A9"/>
@@ -963,96 +1034,205 @@
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="104.44140625" customWidth="1"/>
-    <col min="2" max="2" width="17.33203125" customWidth="1"/>
+    <col min="2" max="2" width="20.21875" customWidth="1"/>
     <col min="3" max="3" width="19.109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="16" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:2">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="16" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:2">
-      <c r="A3" s="1" t="s">
+      <c r="A3" s="16" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B3" s="16" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:2">
-      <c r="A4" s="2" t="s">
+      <c r="A4" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B4" s="16" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="5" spans="1:2">
-      <c r="A5" s="2" t="s">
+      <c r="A5" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="B5" s="14" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="6" spans="1:2">
-      <c r="A6" s="2" t="s">
+      <c r="A6" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="B6" s="3" t="s">
+      <c r="B6" s="14" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="7" spans="1:2">
-      <c r="A7" s="2" t="s">
+      <c r="A7" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="B7" s="3" t="s">
+      <c r="B7" s="14" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="8" spans="1:2">
-      <c r="A8" s="2" t="s">
+      <c r="A8" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="B8" s="3" t="s">
+      <c r="B8" s="14" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="9" spans="1:2">
-      <c r="A9" s="2" t="s">
+      <c r="A9" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="B9" s="3" t="s">
+      <c r="B9" s="14" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="10" spans="1:2">
-      <c r="A10" s="2" t="s">
+      <c r="A10" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="B10" s="3" t="s">
+      <c r="B10" s="14" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="11" spans="1:2">
-      <c r="A11" s="2" t="s">
+      <c r="A11" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="B11" s="3" t="s">
+      <c r="B11" s="14" t="s">
         <v>13</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2">
+      <c r="A12" s="13" t="s">
+        <v>57</v>
+      </c>
+      <c r="B12" s="14" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2">
+      <c r="A13" s="13" t="s">
+        <v>59</v>
+      </c>
+      <c r="B13" s="15"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{433FEB91-5AC9-4747-BA5C-9D3A515258B7}">
+  <dimension ref="A1:A8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4"/>
+  <cols>
+    <col min="1" max="1" width="32.5546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1">
+      <c r="A1" s="17" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1">
+      <c r="A2" s="3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1">
+      <c r="A3" s="3" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1">
+      <c r="A4" s="3" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1">
+      <c r="A5" s="3" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1">
+      <c r="A6" s="3" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1">
+      <c r="A7" s="3" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1">
+      <c r="A8" s="3" t="s">
+        <v>66</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B8D3C429-E8F2-4E15-83BA-89F070043F3C}">
+  <dimension ref="A1:A4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4"/>
+  <cols>
+    <col min="1" max="1" width="18.21875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1">
+      <c r="A1" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1">
+      <c r="A2" s="3" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1">
+      <c r="A3" s="3" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1">
+      <c r="A4" s="3" t="s">
+        <v>70</v>
       </c>
     </row>
   </sheetData>

</xml_diff>